<commit_message>
base de datos para exportar
</commit_message>
<xml_diff>
--- a/ingSoft/DBingsoftav.xlsx
+++ b/ingSoft/DBingsoftav.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ingSoftProy\ingSoft\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="14115" windowHeight="8010"/>
   </bookViews>
@@ -114,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,10 +151,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +164,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -207,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,7 +250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,14 +477,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -573,7 +581,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H17" t="s">
@@ -581,14 +589,14 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="B18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">

</xml_diff>